<commit_message>
Change colors, add remaining cards
</commit_message>
<xml_diff>
--- a/data/allies.xlsx
+++ b/data/allies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -46,6 +46,24 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icon_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sen. Oleg Kasparsky</t>
   </si>
   <si>
@@ -157,10 +175,13 @@
     <t xml:space="preserve">Play on another player</t>
   </si>
   <si>
-    <t xml:space="preserve">Attribute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income – 2</t>
+    <t xml:space="preserve">Single_Attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">money</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">Researcher</t>
@@ -169,7 +190,10 @@
     <t xml:space="preserve">1G2X</t>
   </si>
   <si>
-    <t xml:space="preserve">Peek – 1</t>
+    <t xml:space="preserve">eye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
   </si>
   <si>
     <t xml:space="preserve">Tax Collector</t>
@@ -178,28 +202,22 @@
     <t xml:space="preserve">1R1G1B</t>
   </si>
   <si>
-    <t xml:space="preserve">Income + 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ambassador</t>
   </si>
   <si>
     <t xml:space="preserve">1G</t>
   </si>
   <si>
-    <t xml:space="preserve">Trade – 1</t>
+    <t xml:space="preserve">trade</t>
   </si>
   <si>
     <t xml:space="preserve">Philanthropist</t>
   </si>
   <si>
-    <t xml:space="preserve">Income + 1, Peek – 1</t>
+    <t xml:space="preserve">Double_Attribute</t>
   </si>
   <si>
     <t xml:space="preserve">Merchant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income + 1, Trade – 1</t>
   </si>
 </sst>
 </file>
@@ -299,10 +317,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -335,342 +353,414 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1"/>
       <c r="G6" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="J16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>57</v>
+      <c r="M18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Pixel pushing on events
</commit_message>
<xml_diff>
--- a/data/allies.xlsx
+++ b/data/allies.xlsx
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Tax Collector</t>
   </si>
   <si>
-    <t xml:space="preserve">1R1G1B</t>
+    <t xml:space="preserve">1R1G</t>
   </si>
   <si>
     <t xml:space="preserve">Ambassador</t>
@@ -311,7 +311,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Pixel pushing on allies
</commit_message>
<xml_diff>
--- a/data/allies.xlsx
+++ b/data/allies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -67,15 +67,12 @@
     <t xml:space="preserve">Sen. Oleg Kasparsky</t>
   </si>
   <si>
-    <t xml:space="preserve">2X</t>
+    <t xml:space="preserve">3X</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
   </si>
   <si>
-    <t xml:space="preserve">You now produce</t>
-  </si>
-  <si>
     <t xml:space="preserve">Single_Resource</t>
   </si>
   <si>
@@ -121,7 +118,7 @@
     <t xml:space="preserve">Reverend Bruenner</t>
   </si>
   <si>
-    <t xml:space="preserve">4X</t>
+    <t xml:space="preserve">5X</t>
   </si>
   <si>
     <t xml:space="preserve">RY</t>
@@ -154,7 +151,7 @@
     <t xml:space="preserve">NR</t>
   </si>
   <si>
-    <t xml:space="preserve">Rabble-rouser</t>
+    <t xml:space="preserve">Illegitimate Child</t>
   </si>
   <si>
     <t xml:space="preserve">1N</t>
@@ -311,7 +308,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,249 +370,219 @@
       <c r="C2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="G2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1"/>
       <c r="G6" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="G7" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="G9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="G10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="G11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="G12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="G13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="G14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H14" s="0" t="s">
+      <c r="I14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="J14" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>2</v>
@@ -623,22 +590,22 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="G15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="0" t="s">
+      <c r="J15" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>1</v>
@@ -646,22 +613,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="J16" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>1</v>
@@ -669,22 +636,22 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="G17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="J17" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>1</v>
@@ -692,31 +659,31 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="G18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="I18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="M18" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>1</v>
@@ -724,31 +691,31 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="I19" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
All icons have a white background
</commit_message>
<xml_diff>
--- a/data/allies.xlsx
+++ b/data/allies.xlsx
@@ -178,13 +178,13 @@
     <t xml:space="preserve">eye</t>
   </si>
   <si>
+    <t xml:space="preserve">Tax Collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1R1G</t>
+  </si>
+  <si>
     <t xml:space="preserve">+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tax Collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1R1G</t>
   </si>
   <si>
     <t xml:space="preserve">Ambassador</t>
@@ -308,7 +308,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -605,7 +605,7 @@
         <v>51</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>1</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>3</v>
@@ -628,7 +628,7 @@
         <v>47</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>1</v>
@@ -651,7 +651,7 @@
         <v>57</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>1</v>
@@ -674,7 +674,7 @@
         <v>47</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>1</v>
@@ -706,7 +706,7 @@
         <v>47</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Replace 'peek' with 'ally number'
</commit_message>
<xml_diff>
--- a/data/allies.xlsx
+++ b/data/allies.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Number_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Sen. Oleg Kasparsky</t>
+    <t xml:space="preserve">Senator Dooley</t>
   </si>
   <si>
     <t xml:space="preserve">3X</t>
@@ -76,25 +76,25 @@
     <t xml:space="preserve">Single_Resource</t>
   </si>
   <si>
-    <t xml:space="preserve">Chancellor Knaussman</t>
+    <t xml:space="preserve">Chancellor O’Leary</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Rep. Jans Liskoff</t>
+    <t xml:space="preserve">Representative Wexler</t>
   </si>
   <si>
     <t xml:space="preserve">G</t>
   </si>
   <si>
-    <t xml:space="preserve">Major Cornwallis</t>
+    <t xml:space="preserve">Major Brighton</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">Rep. John Vandermore</t>
+    <t xml:space="preserve">Minister Cartwright</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">1X</t>
   </si>
   <si>
-    <t xml:space="preserve">Reverend Bruenner</t>
+    <t xml:space="preserve">Hon. Rev. Shumacher</t>
   </si>
   <si>
     <t xml:space="preserve">5X</t>
@@ -127,25 +127,25 @@
     <t xml:space="preserve">Double_Resource</t>
   </si>
   <si>
-    <t xml:space="preserve">Lord Otto von Blaylock</t>
+    <t xml:space="preserve">Lord Edwards</t>
   </si>
   <si>
     <t xml:space="preserve">YB</t>
   </si>
   <si>
-    <t xml:space="preserve">Sen. Erik Southstern</t>
+    <t xml:space="preserve">Vice-President Ramsay</t>
   </si>
   <si>
     <t xml:space="preserve">BG</t>
   </si>
   <si>
-    <t xml:space="preserve">Rep. Hunter Olaffsen</t>
+    <t xml:space="preserve">Prime Minister Kramnik</t>
   </si>
   <si>
     <t xml:space="preserve">GN</t>
   </si>
   <si>
-    <t xml:space="preserve">Dr. Lev Kraminsky</t>
+    <t xml:space="preserve">Dr. Leon Schweiss</t>
   </si>
   <si>
     <t xml:space="preserve">NR</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">1G2X</t>
   </si>
   <si>
-    <t xml:space="preserve">eye</t>
+    <t xml:space="preserve">ally_number</t>
   </si>
   <si>
     <t xml:space="preserve">Tax Collector</t>
@@ -308,7 +308,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Move double-attribute stuff side by side
</commit_message>
<xml_diff>
--- a/data/allies.xlsx
+++ b/data/allies.xlsx
@@ -88,13 +88,13 @@
     <t xml:space="preserve">G</t>
   </si>
   <si>
-    <t xml:space="preserve">Major Brighton</t>
+    <t xml:space="preserve">Major Gen. Brighton</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">Minister Cartwright</t>
+    <t xml:space="preserve">Governor Cartwright</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">YB</t>
   </si>
   <si>
-    <t xml:space="preserve">Vice-President Ramsay</t>
+    <t xml:space="preserve">Vice President Ramsey</t>
   </si>
   <si>
     <t xml:space="preserve">BG</t>
@@ -145,13 +145,13 @@
     <t xml:space="preserve">GN</t>
   </si>
   <si>
-    <t xml:space="preserve">Dr. Leon Schweiss</t>
+    <t xml:space="preserve">Dr. Jacob Neumann</t>
   </si>
   <si>
     <t xml:space="preserve">NR</t>
   </si>
   <si>
-    <t xml:space="preserve">Illegitimate Child</t>
+    <t xml:space="preserve">Layabout</t>
   </si>
   <si>
     <t xml:space="preserve">1N</t>
@@ -178,25 +178,22 @@
     <t xml:space="preserve">ally_number</t>
   </si>
   <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tax Collector</t>
   </si>
   <si>
-    <t xml:space="preserve">1R1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+</t>
+    <t xml:space="preserve">1N1R</t>
   </si>
   <si>
     <t xml:space="preserve">Ambassador</t>
   </si>
   <si>
-    <t xml:space="preserve">1G</t>
-  </si>
-  <si>
     <t xml:space="preserve">trade</t>
   </si>
   <si>
-    <t xml:space="preserve">Philanthropist</t>
+    <t xml:space="preserve">Wealthy Donor</t>
   </si>
   <si>
     <t xml:space="preserve">1G3X</t>
@@ -205,7 +202,10 @@
     <t xml:space="preserve">Double_Attribute</t>
   </si>
   <si>
-    <t xml:space="preserve">Merchant</t>
+    <t xml:space="preserve">Captain of Industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1N3X</t>
   </si>
 </sst>
 </file>
@@ -308,7 +308,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -596,7 +596,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>46</v>
@@ -605,7 +605,7 @@
         <v>51</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>1</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>3</v>
@@ -628,10 +628,10 @@
         <v>47</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,7 +639,7 @@
         <v>55</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="G17" s="1" t="n">
         <v>3</v>
@@ -648,7 +648,7 @@
         <v>46</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>48</v>
@@ -659,31 +659,31 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="G18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>47</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>51</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>1</v>
@@ -691,28 +691,28 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="G19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>47</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M19" s="0" t="s">
         <v>48</v>
@@ -724,7 +724,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="0" t="n">
         <f aca="false">SUM(G2:G19)</f>
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix up income icon.  Balance ally vs. event counterparts
</commit_message>
<xml_diff>
--- a/data/allies.xlsx
+++ b/data/allies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -34,12 +34,6 @@
     <t xml:space="preserve">Text</t>
   </si>
   <si>
-    <t xml:space="preserve">Rider Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rider Reward</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
@@ -103,7 +97,7 @@
     <t xml:space="preserve">Bodyguard</t>
   </si>
   <si>
-    <t xml:space="preserve">2B</t>
+    <t xml:space="preserve">1B</t>
   </si>
   <si>
     <t xml:space="preserve">Sacrifice to prevent</t>
@@ -184,7 +178,7 @@
     <t xml:space="preserve">Tax Collector</t>
   </si>
   <si>
-    <t xml:space="preserve">1N1R</t>
+    <t xml:space="preserve">1R1N</t>
   </si>
   <si>
     <t xml:space="preserve">Ambassador</t>
@@ -196,16 +190,13 @@
     <t xml:space="preserve">Wealthy Donor</t>
   </si>
   <si>
-    <t xml:space="preserve">1G3X</t>
+    <t xml:space="preserve">1N2X</t>
   </si>
   <si>
     <t xml:space="preserve">Double_Attribute</t>
   </si>
   <si>
     <t xml:space="preserve">Captain of Industry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1N3X</t>
   </si>
 </sst>
 </file>
@@ -305,15 +296,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,378 +356,365 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="E2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="G6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>26</v>
+      <c r="E7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>29</v>
+      <c r="F8" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="E14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>3</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="0" t="n">
+      <c r="I14" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="K15" s="0" t="n">
+      <c r="I15" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>3</v>
+        <v>52</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I16" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="0" t="n">
+      <c r="I17" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>3</v>
+      <c r="G18" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="N18" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="N19" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="0" t="n">
-        <f aca="false">SUM(G2:G19)</f>
-        <v>38</v>
+        <v>54</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>